<commit_message>
EPBDS-8116 generate implementation for Interface instead of using of proxy object if target interface is used as Datatype
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/BeanInterfaceTest.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/BeanInterfaceTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4954CF-024C-478E-AC80-943CDDEB5200}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B020C7-EB74-419F-A888-7FD7AE210399}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
   <si>
     <t>_PK_</t>
   </si>
@@ -200,6 +200,197 @@
         <scheme val="minor"/>
       </rPr>
       <t>updateAndReturn updateAndReturnTest1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data IChildBean </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>myChildBeanData</t>
+    </r>
+  </si>
+  <si>
+    <t>superField2</t>
+  </si>
+  <si>
+    <t>myBean</t>
+  </si>
+  <si>
+    <t>IMyBean</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method IChildBean </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doSomething</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(IChildBean bean)</t>
+    </r>
+  </si>
+  <si>
+    <t>bean.field1 += "-updated";</t>
+  </si>
+  <si>
+    <t>bean.superField2 *= 100;</t>
+  </si>
+  <si>
+    <t>updateAndReturn(bean.myBean);</t>
+  </si>
+  <si>
+    <t>&gt; myChildBeanData</t>
+  </si>
+  <si>
+    <t>_res_.superField2</t>
+  </si>
+  <si>
+    <t>_res_.myBean.field1</t>
+  </si>
+  <si>
+    <t>_res_.myBean.field2</t>
+  </si>
+  <si>
+    <t>foo-updated</t>
+  </si>
+  <si>
+    <t>bar-updated</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doSomething</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> testDoSomethingIChildBean</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data SomeBean </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>someBeanData</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; someBeanData</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Datatype </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SomeBean</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method SomeBean </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doSomeBean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(SomeBean bean)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Test</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> doSomeBean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> testDoSomethingSomeBean</t>
     </r>
   </si>
 </sst>
@@ -302,13 +493,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,7 +519,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -605,22 +799,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D8"/>
+  <dimension ref="B3:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -642,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>1</v>
       </c>
@@ -653,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -664,7 +864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>3</v>
       </c>
@@ -675,9 +875,142 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>22</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -686,34 +1019,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9942AC7-6F51-46AB-8E61-4915D58192A9}">
-  <dimension ref="B2:D43"/>
+  <dimension ref="B2:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -778,39 +1115,39 @@
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -875,7 +1212,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="11">
+      <c r="B29" s="6">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -886,7 +1223,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="11">
+      <c r="B30" s="6">
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -897,7 +1234,7 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="11">
+      <c r="B31" s="6">
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -908,11 +1245,11 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
@@ -976,17 +1313,219 @@
         <v>30</v>
       </c>
     </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="10"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="10"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
+        <v>2</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" s="2">
+        <v>2200</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="10"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="10"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="10"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="2">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="2">
+        <v>2</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" s="2">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="19">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B64:C64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1007,10 +1546,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">

</xml_diff>